<commit_message>
add runMadden.py to automate testing of rolling training window
</commit_message>
<xml_diff>
--- a/nfl/results.xlsx
+++ b/nfl/results.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="980" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>train</t>
   </si>
@@ -60,15 +61,39 @@
   <si>
     <t>Average of win by</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Sum of win by</t>
+  </si>
+  <si>
+    <t>Winning score</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Spread score</t>
+  </si>
+  <si>
+    <t>margin</t>
+  </si>
+  <si>
+    <t>Average of score</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +117,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -109,8 +142,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -118,37 +224,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -433,7 +553,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" printDrill="1" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" printDrill="1" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -522,10 +642,92 @@
     <dataField name="Average of win by" fld="4" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Average of score" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Sum of win by" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -859,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1115,10 +1317,272 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" thickBot="1">
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" thickBot="1">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4">
+        <v>2008</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1636</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-11</v>
+      </c>
+      <c r="D5">
+        <f>B5-C5</f>
+        <v>1647</v>
+      </c>
+      <c r="F5" s="6">
+        <f>A5</f>
+        <v>2008</v>
+      </c>
+      <c r="G5" s="6">
+        <f>D5</f>
+        <v>1647</v>
+      </c>
+      <c r="H5" s="6">
+        <f>B5</f>
+        <v>1636</v>
+      </c>
+      <c r="I5" s="6">
+        <f>H5-G5</f>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="4">
+        <v>2009</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1708</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D10" si="0">B6-C6</f>
+        <v>1710</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F10" si="1">A6</f>
+        <v>2009</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" ref="G6:G10" si="2">D6</f>
+        <v>1710</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ref="H6:H10" si="3">B6</f>
+        <v>1708</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" ref="I6:I10" si="4">H6-G6</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1593</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1590</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="1"/>
+        <v>2010</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="2"/>
+        <v>1590</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="3"/>
+        <v>1593</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="4">
+        <v>2011</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1691</v>
+      </c>
+      <c r="C8" s="2">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1670</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="1"/>
+        <v>2011</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="2"/>
+        <v>1670</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="3"/>
+        <v>1691</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="4">
+        <v>2012</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1623</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1632</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="1"/>
+        <v>2012</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="2"/>
+        <v>1632</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="3"/>
+        <v>1623</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="4"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="4">
+        <v>2013</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1655</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1651</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="1"/>
+        <v>2013</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="2"/>
+        <v>1651</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="3"/>
+        <v>1655</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1651.5714285714287</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
add section in notebook to predict games
</commit_message>
<xml_diff>
--- a/nfl/results.xlsx
+++ b/nfl/results.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="980" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2080" yWindow="1120" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="35" r:id="rId5"/>
+    <pivotCache cacheId="41" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="27">
   <si>
     <t>train</t>
   </si>
@@ -85,6 +87,27 @@
   <si>
     <t>Average of score</t>
   </si>
+  <si>
+    <t>2010-12</t>
+  </si>
+  <si>
+    <t>2009-11</t>
+  </si>
+  <si>
+    <t>2008-10</t>
+  </si>
+  <si>
+    <t>2007-09</t>
+  </si>
+  <si>
+    <t>2006-08</t>
+  </si>
+  <si>
+    <t>2005-07</t>
+  </si>
+  <si>
+    <t>winScore</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +147,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,7 +255,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -228,8 +267,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -252,21 +309,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -323,6 +427,82 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Amit Bhattacharyya" refreshedDate="41883.945452777778" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="24">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A31:G55" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="train" numFmtId="0">
+      <sharedItems count="6">
+        <s v="2010-12"/>
+        <s v="2009-11"/>
+        <s v="2008-10"/>
+        <s v="2007-09"/>
+        <s v="2006-08"/>
+        <s v="2005-07"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="test" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2008" maxValue="2013" count="6">
+        <n v="2013"/>
+        <n v="2012"/>
+        <n v="2011"/>
+        <n v="2010"/>
+        <n v="2009"/>
+        <n v="2008"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="method" numFmtId="0">
+      <sharedItems count="4">
+        <s v="lineScore"/>
+        <s v="probaScore1"/>
+        <s v="probaScore2"/>
+        <s v="probaScore3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="score" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1593" maxValue="1747"/>
+    </cacheField>
+    <cacheField name="win by" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="-11" maxValue="84" count="20">
+        <n v="2"/>
+        <n v="28"/>
+        <n v="40"/>
+        <n v="35"/>
+        <n v="-9"/>
+        <n v="-2"/>
+        <n v="20"/>
+        <n v="21"/>
+        <n v="49"/>
+        <n v="42"/>
+        <n v="33"/>
+        <n v="3"/>
+        <n v="48"/>
+        <n v="56"/>
+        <n v="37"/>
+        <n v="25"/>
+        <n v="-11"/>
+        <n v="84"/>
+        <n v="77"/>
+        <n v="68"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="win" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="winScore" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1590" maxValue="1710"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="28">
   <r>
@@ -552,8 +732,229 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1655"/>
+    <x v="0"/>
+    <b v="1"/>
+    <n v="1653"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1681"/>
+    <x v="1"/>
+    <b v="1"/>
+    <n v="1653"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="1693"/>
+    <x v="2"/>
+    <b v="1"/>
+    <n v="1653"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="1688"/>
+    <x v="3"/>
+    <b v="1"/>
+    <n v="1653"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1623"/>
+    <x v="4"/>
+    <b v="0"/>
+    <n v="1632"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1630"/>
+    <x v="5"/>
+    <b v="0"/>
+    <n v="1632"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1652"/>
+    <x v="6"/>
+    <b v="1"/>
+    <n v="1632"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1634"/>
+    <x v="0"/>
+    <b v="1"/>
+    <n v="1632"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1691"/>
+    <x v="7"/>
+    <b v="1"/>
+    <n v="1670"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1719"/>
+    <x v="8"/>
+    <b v="1"/>
+    <n v="1670"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="1712"/>
+    <x v="9"/>
+    <b v="1"/>
+    <n v="1670"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1703"/>
+    <x v="10"/>
+    <b v="1"/>
+    <n v="1670"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1593"/>
+    <x v="11"/>
+    <b v="1"/>
+    <n v="1590"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1638"/>
+    <x v="12"/>
+    <b v="1"/>
+    <n v="1590"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="1646"/>
+    <x v="13"/>
+    <b v="1"/>
+    <n v="1590"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1646"/>
+    <x v="13"/>
+    <b v="1"/>
+    <n v="1590"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1708"/>
+    <x v="5"/>
+    <b v="0"/>
+    <n v="1710"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1747"/>
+    <x v="14"/>
+    <b v="1"/>
+    <n v="1710"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="1735"/>
+    <x v="15"/>
+    <b v="1"/>
+    <n v="1710"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="1743"/>
+    <x v="10"/>
+    <b v="1"/>
+    <n v="1710"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1636"/>
+    <x v="16"/>
+    <b v="0"/>
+    <n v="1647"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1731"/>
+    <x v="17"/>
+    <b v="1"/>
+    <n v="1647"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1724"/>
+    <x v="18"/>
+    <b v="1"/>
+    <n v="1647"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1715"/>
+    <x v="19"/>
+    <b v="1"/>
+    <n v="1647"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" printDrill="1" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" printDrill="1" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G12" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -642,7 +1043,7 @@
     <dataField name="Average of win by" fld="4" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="8">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -656,7 +1057,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -728,6 +1129,146 @@
     <dataField name="Average of score" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Sum of win by" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0">
+      <items count="21">
+        <item x="16"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="15"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="14"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of win by" fld="4" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="6">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1062,7 +1603,7 @@
   <dimension ref="A3:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G15" sqref="A1:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1307,6 +1848,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1319,7 +1861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1579,10 +2121,462 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A3:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>2008</v>
+      </c>
+      <c r="C5" s="14">
+        <v>-11</v>
+      </c>
+      <c r="D5" s="14">
+        <v>84</v>
+      </c>
+      <c r="E5" s="14">
+        <v>77</v>
+      </c>
+      <c r="F5" s="14">
+        <v>68</v>
+      </c>
+      <c r="G5" s="14">
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>2009</v>
+      </c>
+      <c r="C6" s="14">
+        <v>-2</v>
+      </c>
+      <c r="D6" s="14">
+        <v>37</v>
+      </c>
+      <c r="E6" s="14">
+        <v>25</v>
+      </c>
+      <c r="F6" s="14">
+        <v>33</v>
+      </c>
+      <c r="G6" s="14">
+        <v>23.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>2010</v>
+      </c>
+      <c r="C7" s="14">
+        <v>3</v>
+      </c>
+      <c r="D7" s="14">
+        <v>48</v>
+      </c>
+      <c r="E7" s="14">
+        <v>56</v>
+      </c>
+      <c r="F7" s="14">
+        <v>56</v>
+      </c>
+      <c r="G7" s="14">
+        <v>40.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>2011</v>
+      </c>
+      <c r="C8" s="14">
+        <v>21</v>
+      </c>
+      <c r="D8" s="14">
+        <v>49</v>
+      </c>
+      <c r="E8" s="14">
+        <v>42</v>
+      </c>
+      <c r="F8" s="14">
+        <v>33</v>
+      </c>
+      <c r="G8" s="14">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>2012</v>
+      </c>
+      <c r="C9" s="14">
+        <v>-9</v>
+      </c>
+      <c r="D9" s="14">
+        <v>-2</v>
+      </c>
+      <c r="E9" s="14">
+        <v>20</v>
+      </c>
+      <c r="F9" s="14">
+        <v>2</v>
+      </c>
+      <c r="G9" s="14">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>2013</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2</v>
+      </c>
+      <c r="D10" s="14">
+        <v>28</v>
+      </c>
+      <c r="E10" s="14">
+        <v>40</v>
+      </c>
+      <c r="F10" s="14">
+        <v>35</v>
+      </c>
+      <c r="G10" s="14">
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D11" s="3">
+        <v>40.666666666666664</v>
+      </c>
+      <c r="E11" s="3">
+        <v>43.333333333333336</v>
+      </c>
+      <c r="F11" s="3">
+        <v>37.833333333333336</v>
+      </c>
+      <c r="G11" s="14">
+        <v>30.625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" s="3">
+        <f>STDEV(C5:C10)</f>
+        <v>11.465891446663303</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ref="D12:F12" si="0">STDEV(D5:D10)</f>
+        <v>28.267767274170538</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>20.915703829100917</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>22.710496838833507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20">
+        <v>2008</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-11</v>
+      </c>
+      <c r="D20" s="2">
+        <v>90</v>
+      </c>
+      <c r="E20" s="2">
+        <v>71</v>
+      </c>
+      <c r="F20" s="2">
+        <v>77</v>
+      </c>
+      <c r="G20" s="2">
+        <v>56.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21">
+        <v>2009</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2">
+        <v>25</v>
+      </c>
+      <c r="F21" s="2">
+        <v>28</v>
+      </c>
+      <c r="G21" s="2">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>2013</v>
+      </c>
+      <c r="B22">
+        <v>2010</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>42</v>
+      </c>
+      <c r="E22" s="2">
+        <v>30</v>
+      </c>
+      <c r="F22" s="2">
+        <v>49</v>
+      </c>
+      <c r="G22" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>2013</v>
+      </c>
+      <c r="B23">
+        <v>2011</v>
+      </c>
+      <c r="C23" s="2">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>2013</v>
+      </c>
+      <c r="B24">
+        <v>2012</v>
+      </c>
+      <c r="C24" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2">
+        <v>42</v>
+      </c>
+      <c r="F24" s="2">
+        <v>15</v>
+      </c>
+      <c r="G24" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>2013</v>
+      </c>
+      <c r="B25">
+        <v>2013</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>47</v>
+      </c>
+      <c r="E25" s="2">
+        <v>77</v>
+      </c>
+      <c r="F25" s="2">
+        <v>56</v>
+      </c>
+      <c r="G25" s="2">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="D26" s="3">
+        <v>33.714285714285715</v>
+      </c>
+      <c r="E26" s="3">
+        <v>37.571428571428569</v>
+      </c>
+      <c r="F26" s="3">
+        <v>32.714285714285715</v>
+      </c>
+      <c r="G26" s="3">
+        <v>26.214285714285715</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="C28" s="3">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="D28" s="3">
+        <v>33.714285714285715</v>
+      </c>
+      <c r="E28" s="3">
+        <v>37.571428571428569</v>
+      </c>
+      <c r="F28" s="3">
+        <v>32.714285714285715</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="C29" s="3">
+        <v>10.47900395121234</v>
+      </c>
+      <c r="D29" s="3">
+        <v>29.533677306392025</v>
+      </c>
+      <c r="E29" s="3">
+        <v>27.657772523332046</v>
+      </c>
+      <c r="F29" s="3">
+        <v>28.894718581511775</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1907,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -1927,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -1947,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>2013</v>
       </c>
@@ -1967,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -1987,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>2013</v>
       </c>
@@ -2007,7 +3001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>2013</v>
       </c>
@@ -2027,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>2013</v>
       </c>
@@ -2047,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>2013</v>
       </c>
@@ -2067,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -2087,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2012</v>
       </c>
@@ -2107,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>2012</v>
       </c>
@@ -2127,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>2012</v>
       </c>
@@ -2147,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>2012</v>
       </c>
@@ -2166,6 +3160,653 @@
       <c r="F29" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <v>2013</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>1655</v>
+      </c>
+      <c r="E32">
+        <f>D32-G32</f>
+        <v>2</v>
+      </c>
+      <c r="F32" t="b">
+        <f>E32&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="19">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>2013</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>1681</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ref="E33:E55" si="0">D33-G33</f>
+        <v>28</v>
+      </c>
+      <c r="F33" t="b">
+        <f t="shared" ref="F33:F55" si="1">E33&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1653</v>
+      </c>
+      <c r="J33" s="12"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="11"/>
+    </row>
+    <row r="34" spans="1:12" ht="19">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>2013</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>1693</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F34" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1653</v>
+      </c>
+      <c r="J34" s="12"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="11"/>
+    </row>
+    <row r="35" spans="1:12" ht="19">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>2013</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>1688</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="F35" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1653</v>
+      </c>
+      <c r="J35" s="12"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="11"/>
+    </row>
+    <row r="36" spans="1:12" ht="19">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <v>2012</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>1623</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="F36" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="11">
+        <v>1632</v>
+      </c>
+      <c r="J36" s="12"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="11"/>
+    </row>
+    <row r="37" spans="1:12" ht="19">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <v>2012</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>1630</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="F37" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="11">
+        <v>1632</v>
+      </c>
+      <c r="J37" s="12"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="19">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>2012</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>1652</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F38" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G38" s="11">
+        <v>1632</v>
+      </c>
+      <c r="J38" s="12"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="11"/>
+    </row>
+    <row r="39" spans="1:12" ht="19">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39">
+        <v>2012</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>1634</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F39" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G39" s="11">
+        <v>1632</v>
+      </c>
+      <c r="J39" s="12"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="11"/>
+    </row>
+    <row r="40" spans="1:12" ht="18">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40">
+        <v>2011</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>1691</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F40" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G40" s="11">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="18">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41">
+        <v>2011</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>1719</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="F41" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G41" s="11">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="18">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42">
+        <v>2011</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>1712</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="F42" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G42" s="11">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="18">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43">
+        <v>2011</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>1703</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="F43" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G43" s="11">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="18">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44">
+        <v>2010</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1593</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F44" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G44" s="11">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="18">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>2010</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>1638</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F45" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G45" s="11">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="18">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <v>2010</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>1646</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="F46" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G46" s="11">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="18">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47">
+        <v>2010</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>1646</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="F47" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G47" s="11">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="18">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48">
+        <v>2009</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>1708</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="F48" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="11">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49">
+        <v>2009</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>1747</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="F49" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G49" s="11">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>2009</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>1735</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="F50" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G50" s="11">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51">
+        <v>2009</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>1743</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="F51" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G51" s="11">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52">
+        <v>2008</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>1636</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="F52" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="11">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53">
+        <v>2008</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>1731</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="F53" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G53" s="11">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="18">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54">
+        <v>2008</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>1724</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="F54" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G54" s="11">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="18">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55">
+        <v>2008</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>1715</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="F55" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G55" s="11">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17">
+      <c r="C56" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>